<commit_message>
fixed naming ussue that prevented emergency alerting
</commit_message>
<xml_diff>
--- a/src/results.xlsx
+++ b/src/results.xlsx
@@ -510,12 +510,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[258]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[258]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -574,12 +574,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[429]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[429]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">

</xml_diff>

<commit_message>
full working main.py -> pose classifier implemented
</commit_message>
<xml_diff>
--- a/src/results.xlsx
+++ b/src/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>fall1</t>
+          <t>person_laying_but_ok_1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[200]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -500,22 +500,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>fal6_cropped</t>
+          <t>simulation_proximus_2_fall_in_line_with_cam_view</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[400]</t>
+          <t>[135]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[258]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[258]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -532,12 +532,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Stroke_Simulation_1</t>
+          <t>person_laying_but_ok_2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[250]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -564,22 +564,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FallingAwayFromCamera</t>
+          <t>simulation_chantier_2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[220]</t>
+          <t>[700]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[429]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[429]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -596,12 +596,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Stroke_Simulation_2</t>
+          <t>young_man_living_2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[200]</t>
+          <t>[340]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -628,12 +628,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FallBehindObject</t>
+          <t>person_laying_but_ok_3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[100]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -654,6 +654,70 @@
       <c r="F7" t="inlineStr">
         <is>
           <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>person_laying_but_ok_4</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>young_man_watching_tv</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[339]</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>[339]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
full integration yolo pose + new results
</commit_message>
<xml_diff>
--- a/src/results.xlsx
+++ b/src/results.xlsx
@@ -862,7 +862,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[273]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[273]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[495]</t>
+          <t>[330]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[495]</t>
+          <t>[330]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[312]</t>
+          <t>[327]</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1118,12 +1118,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[348]</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[170]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[170]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[132]</t>
+          <t>[192]</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">

</xml_diff>

<commit_message>
fixed some bugs as per usual
</commit_message>
<xml_diff>
--- a/src/results.xlsx
+++ b/src/results.xlsx
@@ -830,7 +830,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[234]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -840,7 +840,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[234]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[330]</t>
+          <t>[336]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[330]</t>
+          <t>[336]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -990,22 +990,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[186]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>[90]</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[606]</t>
+          <t>[585]</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1054,22 +1054,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[795]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>[700]</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1086,22 +1086,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[327]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>[260]</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1118,22 +1118,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[348]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>[170]</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1182,22 +1182,22 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[312]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>[340]</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[447]</t>
+          <t>[483]</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[342]</t>
+          <t>[375]</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[270]</t>
+          <t>[291]</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[192]</t>
+          <t>[150]</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1406,12 +1406,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[375]</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[300]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[300]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1470,22 +1470,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[711]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
           <t>[600]</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[468]</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[468]</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>[228]</t>
+          <t>[213]</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[180]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[180]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[258]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[258]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[225]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[225]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">

</xml_diff>